<commit_message>
Add draft for vectorized results extraction
TODO: Tidy up and integrate! :-)
</commit_message>
<xml_diff>
--- a/Columns.xlsx
+++ b/Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\DR_mod\DR_Potentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF308BD-34F0-4B1E-BF08-4CE087B90E29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7493B726-FFA1-4514-BDF5-FBDC1D44FCBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="432">
   <si>
     <t>Gruppe</t>
   </si>
@@ -1295,54 +1295,6 @@
   </si>
   <si>
     <t>drop</t>
-  </si>
-  <si>
-    <t>Fundstelle Maximallast</t>
-  </si>
-  <si>
-    <t>Fundstelle Minimalauslastung</t>
-  </si>
-  <si>
-    <t>Fundstelle Minimallast</t>
-  </si>
-  <si>
-    <t>Fundstelle Potenzial negativ Mittel</t>
-  </si>
-  <si>
-    <t>Fundstelle Potenzial negativ min</t>
-  </si>
-  <si>
-    <t>Fundstelle Potenzial negativ max</t>
-  </si>
-  <si>
-    <t>Fundstelle Potenzial positiv Mittel</t>
-  </si>
-  <si>
-    <t>Fundstelle Potenzial positiv min</t>
-  </si>
-  <si>
-    <t>Fundstelle Potenzial positiv max</t>
-  </si>
-  <si>
-    <t>Fundstelle Schaltdauer positiv</t>
-  </si>
-  <si>
-    <t>Fundstelle Schaltdauer negativ</t>
-  </si>
-  <si>
-    <t>Fundstelle Durchschnittsleistung</t>
-  </si>
-  <si>
-    <t>Fundstelle maximale Abrufhäufigkeit pro Jahr</t>
-  </si>
-  <si>
-    <t>Fundstelle maximale Abrufhäufigkeit pro Woche</t>
-  </si>
-  <si>
-    <t>Fundstelle variable Kosten</t>
-  </si>
-  <si>
-    <t>Fundstelle flexibilisierbarer Leistungsanteil</t>
   </si>
   <si>
     <t>max</t>
@@ -1570,9 +1522,9 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{354C2B9C-026C-4A8E-BFA8-A99211BC8AE4}" name="Spaltenname" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2971FB75-8976-49B2-8AA0-40D58A8C0143}" name="Gruppe" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DC746ADC-2D8C-4D9E-AF3F-474CC8C65D87}" name="Numerisch?" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{AB80D3B8-0003-48F6-8701-E0CEE270263C}" name="Verzicht / Verschiebung / nicht spezifiziert" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{3E84D8F4-A1D1-4685-92DE-F4B7F6FDBBBB}" name="Aggregationsregel" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{DC746ADC-2D8C-4D9E-AF3F-474CC8C65D87}" name="Numerisch?" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AB80D3B8-0003-48F6-8701-E0CEE270263C}" name="Verzicht / Verschiebung / nicht spezifiziert" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3E84D8F4-A1D1-4685-92DE-F4B7F6FDBBBB}" name="Aggregationsregel" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1901,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
-      <selection activeCell="C390" sqref="C390"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>421</v>
@@ -1939,10 +1891,10 @@
         <v>387</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>422</v>
@@ -1956,10 +1908,10 @@
         <v>387</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>422</v>
@@ -1973,10 +1925,10 @@
         <v>387</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>422</v>
@@ -1990,10 +1942,10 @@
         <v>387</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>422</v>
@@ -2007,10 +1959,10 @@
         <v>387</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>422</v>
@@ -2024,10 +1976,10 @@
         <v>387</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>422</v>
@@ -2041,10 +1993,10 @@
         <v>387</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>422</v>
@@ -2058,10 +2010,10 @@
         <v>387</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>422</v>
@@ -2075,10 +2027,10 @@
         <v>387</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>422</v>
@@ -2092,7 +2044,7 @@
         <v>388</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>417</v>
@@ -2109,10 +2061,10 @@
         <v>389</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>424</v>
@@ -2126,10 +2078,10 @@
         <v>389</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>424</v>
@@ -2143,10 +2095,10 @@
         <v>389</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>424</v>
@@ -2160,10 +2112,10 @@
         <v>389</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>424</v>
@@ -2177,10 +2129,10 @@
         <v>389</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>424</v>
@@ -2194,10 +2146,10 @@
         <v>389</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>424</v>
@@ -2211,10 +2163,10 @@
         <v>389</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>424</v>
@@ -2228,10 +2180,10 @@
         <v>390</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>422</v>
@@ -2245,10 +2197,10 @@
         <v>391</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>422</v>
@@ -2262,10 +2214,10 @@
         <v>389</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>424</v>
@@ -2279,10 +2231,10 @@
         <v>392</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>422</v>
@@ -2296,10 +2248,10 @@
         <v>392</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>422</v>
@@ -2313,10 +2265,10 @@
         <v>392</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>422</v>
@@ -2330,10 +2282,10 @@
         <v>392</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>422</v>
@@ -2347,10 +2299,10 @@
         <v>392</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>422</v>
@@ -2364,10 +2316,10 @@
         <v>392</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>422</v>
@@ -2381,10 +2333,10 @@
         <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>422</v>
@@ -2398,10 +2350,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>422</v>
@@ -2415,10 +2367,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>422</v>
@@ -2432,10 +2384,10 @@
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>422</v>
@@ -2449,10 +2401,10 @@
         <v>28</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>422</v>
@@ -2466,10 +2418,10 @@
         <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>422</v>
@@ -2483,10 +2435,10 @@
         <v>28</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>422</v>
@@ -2500,10 +2452,10 @@
         <v>28</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>422</v>
@@ -2517,10 +2469,10 @@
         <v>28</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>422</v>
@@ -2534,10 +2486,10 @@
         <v>28</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>422</v>
@@ -2551,10 +2503,10 @@
         <v>28</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>422</v>
@@ -2568,10 +2520,10 @@
         <v>28</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>422</v>
@@ -2585,10 +2537,10 @@
         <v>28</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>422</v>
@@ -2602,10 +2554,10 @@
         <v>28</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>422</v>
@@ -2619,10 +2571,10 @@
         <v>28</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>422</v>
@@ -2636,10 +2588,10 @@
         <v>28</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>422</v>
@@ -2653,10 +2605,10 @@
         <v>28</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>422</v>
@@ -2670,10 +2622,10 @@
         <v>28</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>422</v>
@@ -2687,10 +2639,10 @@
         <v>28</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>422</v>
@@ -2704,10 +2656,10 @@
         <v>28</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>422</v>
@@ -2721,10 +2673,10 @@
         <v>28</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>422</v>
@@ -2738,10 +2690,10 @@
         <v>28</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>422</v>
@@ -2755,10 +2707,10 @@
         <v>28</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>422</v>
@@ -2772,10 +2724,10 @@
         <v>28</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>422</v>
@@ -2789,10 +2741,10 @@
         <v>28</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>422</v>
@@ -2806,10 +2758,10 @@
         <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>422</v>
@@ -2823,10 +2775,10 @@
         <v>28</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>422</v>
@@ -2840,10 +2792,10 @@
         <v>28</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>422</v>
@@ -2857,10 +2809,10 @@
         <v>28</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>422</v>
@@ -2874,10 +2826,10 @@
         <v>28</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>422</v>
@@ -2891,10 +2843,10 @@
         <v>28</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>422</v>
@@ -2908,10 +2860,10 @@
         <v>28</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>422</v>
@@ -2925,10 +2877,10 @@
         <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>422</v>
@@ -2942,10 +2894,10 @@
         <v>28</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>422</v>
@@ -2959,10 +2911,10 @@
         <v>389</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>424</v>
@@ -2976,10 +2928,10 @@
         <v>389</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>424</v>
@@ -2993,10 +2945,10 @@
         <v>389</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>424</v>
@@ -3010,10 +2962,10 @@
         <v>387</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>423</v>
@@ -3027,10 +2979,10 @@
         <v>388</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>423</v>
@@ -3044,10 +2996,10 @@
         <v>389</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>423</v>
@@ -3061,10 +3013,10 @@
         <v>389</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>423</v>
@@ -3078,10 +3030,10 @@
         <v>389</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>423</v>
@@ -3095,10 +3047,10 @@
         <v>390</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>423</v>
@@ -3112,10 +3064,10 @@
         <v>391</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>423</v>
@@ -3129,10 +3081,10 @@
         <v>28</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>423</v>
@@ -3146,10 +3098,10 @@
         <v>389</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>423</v>
@@ -3163,10 +3115,10 @@
         <v>393</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>423</v>
@@ -3180,10 +3132,10 @@
         <v>389</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>423</v>
@@ -3194,13 +3146,13 @@
         <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>423</v>
@@ -3211,13 +3163,13 @@
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>423</v>
@@ -3228,13 +3180,13 @@
         <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>423</v>
@@ -3245,13 +3197,13 @@
         <v>79</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>425</v>
+        <v>394</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>423</v>
@@ -3262,13 +3214,13 @@
         <v>80</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>423</v>
@@ -3279,13 +3231,13 @@
         <v>81</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>423</v>
@@ -3296,10 +3248,10 @@
         <v>82</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>417</v>
@@ -3313,10 +3265,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>417</v>
@@ -3330,10 +3282,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>417</v>
@@ -3347,13 +3299,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
+        <v>398</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>423</v>
@@ -3364,13 +3316,13 @@
         <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>423</v>
@@ -3381,13 +3333,13 @@
         <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>423</v>
@@ -3401,10 +3353,10 @@
         <v>389</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>423</v>
@@ -3415,13 +3367,13 @@
         <v>85</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>85</v>
+        <v>399</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>423</v>
@@ -3432,13 +3384,13 @@
         <v>86</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>434</v>
+        <v>400</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>423</v>
@@ -3449,10 +3401,10 @@
         <v>86</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>417</v>
@@ -3466,13 +3418,13 @@
         <v>87</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>87</v>
+        <v>401</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>423</v>
@@ -3483,10 +3435,10 @@
         <v>88</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>88</v>
+        <v>402</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>417</v>
@@ -3500,13 +3452,13 @@
         <v>89</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>91</v>
+        <v>391</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>423</v>
@@ -3517,13 +3469,13 @@
         <v>90</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>90</v>
+        <v>403</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>423</v>
@@ -3534,13 +3486,13 @@
         <v>91</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>91</v>
+        <v>391</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>423</v>
@@ -3551,13 +3503,13 @@
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>423</v>
@@ -3568,13 +3520,13 @@
         <v>93</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>436</v>
+        <v>392</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>423</v>
@@ -3585,13 +3537,13 @@
         <v>94</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>94</v>
+        <v>390</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>423</v>
@@ -3602,13 +3554,13 @@
         <v>96</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>96</v>
+        <v>405</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>423</v>
@@ -3619,13 +3571,13 @@
         <v>97</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>437</v>
+        <v>406</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>423</v>
@@ -3636,13 +3588,13 @@
         <v>97</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>423</v>
@@ -3653,13 +3605,13 @@
         <v>98</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>439</v>
+        <v>388</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>423</v>
@@ -3673,10 +3625,10 @@
         <v>389</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>423</v>
@@ -3690,10 +3642,10 @@
         <v>389</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>423</v>
@@ -3704,13 +3656,13 @@
         <v>95</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>440</v>
+        <v>404</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>423</v>
@@ -3724,10 +3676,10 @@
         <v>389</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>424</v>
@@ -3741,10 +3693,10 @@
         <v>389</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>424</v>
@@ -3758,10 +3710,10 @@
         <v>393</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>422</v>
@@ -3775,13 +3727,13 @@
         <v>104</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3792,13 +3744,13 @@
         <v>389</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,13 +3761,13 @@
         <v>106</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3826,13 +3778,13 @@
         <v>107</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>417</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3843,13 +3795,13 @@
         <v>108</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>418</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3860,10 +3812,10 @@
         <v>109</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>422</v>
@@ -3877,10 +3829,10 @@
         <v>109</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>422</v>
@@ -3894,10 +3846,10 @@
         <v>109</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>422</v>
@@ -3911,10 +3863,10 @@
         <v>109</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>422</v>
@@ -3928,10 +3880,10 @@
         <v>394</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>422</v>
@@ -3945,10 +3897,10 @@
         <v>394</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>422</v>
@@ -3962,10 +3914,10 @@
         <v>394</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>422</v>
@@ -3979,10 +3931,10 @@
         <v>394</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>422</v>
@@ -3996,10 +3948,10 @@
         <v>394</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>422</v>
@@ -4013,10 +3965,10 @@
         <v>394</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>422</v>
@@ -4030,10 +3982,10 @@
         <v>394</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>422</v>
@@ -4047,10 +3999,10 @@
         <v>394</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>422</v>
@@ -4064,10 +4016,10 @@
         <v>395</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>422</v>
@@ -4081,10 +4033,10 @@
         <v>395</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>422</v>
@@ -4098,10 +4050,10 @@
         <v>395</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>422</v>
@@ -4115,10 +4067,10 @@
         <v>395</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>422</v>
@@ -4132,10 +4084,10 @@
         <v>396</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>422</v>
@@ -4149,10 +4101,10 @@
         <v>396</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>422</v>
@@ -4166,10 +4118,10 @@
         <v>396</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>422</v>
@@ -4183,10 +4135,10 @@
         <v>396</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>422</v>
@@ -4200,10 +4152,10 @@
         <v>398</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>423</v>
@@ -4217,7 +4169,7 @@
         <v>397</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>417</v>
@@ -4234,7 +4186,7 @@
         <v>397</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>417</v>
@@ -4251,7 +4203,7 @@
         <v>397</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>417</v>
@@ -4268,7 +4220,7 @@
         <v>397</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>417</v>
@@ -4285,7 +4237,7 @@
         <v>397</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>417</v>
@@ -4302,7 +4254,7 @@
         <v>397</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>417</v>
@@ -4319,7 +4271,7 @@
         <v>397</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>417</v>
@@ -4336,7 +4288,7 @@
         <v>397</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>417</v>
@@ -4353,7 +4305,7 @@
         <v>397</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>417</v>
@@ -4370,7 +4322,7 @@
         <v>397</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>417</v>
@@ -4387,7 +4339,7 @@
         <v>397</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>417</v>
@@ -4404,7 +4356,7 @@
         <v>397</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>417</v>
@@ -4421,7 +4373,7 @@
         <v>397</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>417</v>
@@ -4438,7 +4390,7 @@
         <v>397</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>417</v>
@@ -4455,7 +4407,7 @@
         <v>407</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>417</v>
@@ -4472,7 +4424,7 @@
         <v>407</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>417</v>
@@ -4489,7 +4441,7 @@
         <v>407</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>417</v>
@@ -4506,7 +4458,7 @@
         <v>407</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>417</v>
@@ -4523,7 +4475,7 @@
         <v>407</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>417</v>
@@ -4540,7 +4492,7 @@
         <v>407</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>417</v>
@@ -4557,7 +4509,7 @@
         <v>407</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>417</v>
@@ -4574,7 +4526,7 @@
         <v>407</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>417</v>
@@ -4591,7 +4543,7 @@
         <v>407</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>417</v>
@@ -4608,7 +4560,7 @@
         <v>408</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>417</v>
@@ -4625,7 +4577,7 @@
         <v>408</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>417</v>
@@ -4642,7 +4594,7 @@
         <v>408</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>417</v>
@@ -4659,7 +4611,7 @@
         <v>408</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>417</v>
@@ -4676,7 +4628,7 @@
         <v>408</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>417</v>
@@ -4693,7 +4645,7 @@
         <v>408</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>417</v>
@@ -4710,7 +4662,7 @@
         <v>408</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>417</v>
@@ -4727,7 +4679,7 @@
         <v>408</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>417</v>
@@ -4744,7 +4696,7 @@
         <v>408</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>417</v>
@@ -4761,7 +4713,7 @@
         <v>397</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>417</v>
@@ -4778,7 +4730,7 @@
         <v>397</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>417</v>
@@ -4795,7 +4747,7 @@
         <v>397</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>417</v>
@@ -4812,7 +4764,7 @@
         <v>397</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>417</v>
@@ -4829,7 +4781,7 @@
         <v>397</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>417</v>
@@ -4846,7 +4798,7 @@
         <v>389</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>417</v>
@@ -4863,7 +4815,7 @@
         <v>407</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>417</v>
@@ -4880,7 +4832,7 @@
         <v>407</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>417</v>
@@ -4897,7 +4849,7 @@
         <v>407</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>417</v>
@@ -4914,7 +4866,7 @@
         <v>407</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>417</v>
@@ -4931,7 +4883,7 @@
         <v>407</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>417</v>
@@ -4948,7 +4900,7 @@
         <v>408</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>417</v>
@@ -4965,7 +4917,7 @@
         <v>408</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>417</v>
@@ -4982,7 +4934,7 @@
         <v>398</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>418</v>
@@ -4999,7 +4951,7 @@
         <v>398</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>417</v>
@@ -5016,7 +4968,7 @@
         <v>398</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>417</v>
@@ -5033,7 +4985,7 @@
         <v>398</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>417</v>
@@ -5050,7 +5002,7 @@
         <v>414</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>418</v>
@@ -5067,7 +5019,7 @@
         <v>398</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>417</v>
@@ -5084,7 +5036,7 @@
         <v>398</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>417</v>
@@ -5101,7 +5053,7 @@
         <v>398</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>417</v>
@@ -5118,7 +5070,7 @@
         <v>414</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>418</v>
@@ -5135,7 +5087,7 @@
         <v>398</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>417</v>
@@ -5152,7 +5104,7 @@
         <v>414</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>418</v>
@@ -5169,7 +5121,7 @@
         <v>398</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>417</v>
@@ -5186,7 +5138,7 @@
         <v>415</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>418</v>
@@ -5203,7 +5155,7 @@
         <v>398</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>417</v>
@@ -5220,7 +5172,7 @@
         <v>398</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>417</v>
@@ -5237,7 +5189,7 @@
         <v>414</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>418</v>
@@ -5254,7 +5206,7 @@
         <v>398</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>417</v>
@@ -5271,7 +5223,7 @@
         <v>414</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>418</v>
@@ -5288,7 +5240,7 @@
         <v>398</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>417</v>
@@ -5305,7 +5257,7 @@
         <v>414</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>418</v>
@@ -5322,7 +5274,7 @@
         <v>398</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>417</v>
@@ -5339,7 +5291,7 @@
         <v>414</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>418</v>
@@ -5356,7 +5308,7 @@
         <v>398</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>417</v>
@@ -5373,7 +5325,7 @@
         <v>414</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>418</v>
@@ -5390,7 +5342,7 @@
         <v>409</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>417</v>
@@ -5407,7 +5359,7 @@
         <v>409</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>417</v>
@@ -5424,7 +5376,7 @@
         <v>415</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>418</v>
@@ -5441,7 +5393,7 @@
         <v>409</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>417</v>
@@ -5458,7 +5410,7 @@
         <v>415</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>418</v>
@@ -5475,7 +5427,7 @@
         <v>409</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>417</v>
@@ -5492,7 +5444,7 @@
         <v>415</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>418</v>
@@ -5509,7 +5461,7 @@
         <v>409</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>417</v>
@@ -5526,7 +5478,7 @@
         <v>415</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>418</v>
@@ -5543,7 +5495,7 @@
         <v>409</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>417</v>
@@ -5560,7 +5512,7 @@
         <v>415</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>418</v>
@@ -5577,7 +5529,7 @@
         <v>409</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>417</v>
@@ -5594,7 +5546,7 @@
         <v>415</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>418</v>
@@ -5611,7 +5563,7 @@
         <v>409</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>417</v>
@@ -5628,7 +5580,7 @@
         <v>415</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>418</v>
@@ -5645,7 +5597,7 @@
         <v>409</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>417</v>
@@ -5662,7 +5614,7 @@
         <v>415</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>418</v>
@@ -5679,7 +5631,7 @@
         <v>410</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>417</v>
@@ -5696,7 +5648,7 @@
         <v>410</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>417</v>
@@ -5713,7 +5665,7 @@
         <v>416</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>418</v>
@@ -5730,7 +5682,7 @@
         <v>410</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>417</v>
@@ -5747,7 +5699,7 @@
         <v>416</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>418</v>
@@ -5764,7 +5716,7 @@
         <v>410</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>417</v>
@@ -5781,7 +5733,7 @@
         <v>416</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>418</v>
@@ -5798,7 +5750,7 @@
         <v>410</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>417</v>
@@ -5815,7 +5767,7 @@
         <v>416</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>418</v>
@@ -5832,7 +5784,7 @@
         <v>410</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>417</v>
@@ -5849,7 +5801,7 @@
         <v>416</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>418</v>
@@ -5866,7 +5818,7 @@
         <v>410</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>417</v>
@@ -5883,7 +5835,7 @@
         <v>416</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>418</v>
@@ -5900,7 +5852,7 @@
         <v>410</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>417</v>
@@ -5917,7 +5869,7 @@
         <v>416</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>418</v>
@@ -5934,7 +5886,7 @@
         <v>410</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>417</v>
@@ -5951,7 +5903,7 @@
         <v>416</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>418</v>
@@ -5968,7 +5920,7 @@
         <v>398</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>417</v>
@@ -5985,7 +5937,7 @@
         <v>416</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>418</v>
@@ -6002,7 +5954,7 @@
         <v>398</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>417</v>
@@ -6019,7 +5971,7 @@
         <v>416</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>418</v>
@@ -6036,7 +5988,7 @@
         <v>398</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>417</v>
@@ -6053,7 +6005,7 @@
         <v>416</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>418</v>
@@ -6070,7 +6022,7 @@
         <v>398</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>417</v>
@@ -6087,7 +6039,7 @@
         <v>398</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>417</v>
@@ -6104,7 +6056,7 @@
         <v>389</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>417</v>
@@ -6121,7 +6073,7 @@
         <v>409</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>417</v>
@@ -6138,7 +6090,7 @@
         <v>415</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>417</v>
@@ -6155,7 +6107,7 @@
         <v>409</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>418</v>
@@ -6172,7 +6124,7 @@
         <v>409</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>417</v>
@@ -6189,7 +6141,7 @@
         <v>409</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>417</v>
@@ -6206,7 +6158,7 @@
         <v>415</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>418</v>
@@ -6223,7 +6175,7 @@
         <v>409</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>417</v>
@@ -6240,7 +6192,7 @@
         <v>409</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>417</v>
@@ -6257,7 +6209,7 @@
         <v>410</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>417</v>
@@ -6274,7 +6226,7 @@
         <v>416</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>418</v>
@@ -6291,7 +6243,7 @@
         <v>410</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D258" s="2" t="s">
         <v>417</v>
@@ -6308,10 +6260,10 @@
         <v>253</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E259" s="2" t="s">
         <v>424</v>
@@ -6325,10 +6277,10 @@
         <v>399</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E260" s="2" t="s">
         <v>424</v>
@@ -6342,10 +6294,10 @@
         <v>399</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E261" s="2" t="s">
         <v>424</v>
@@ -6359,10 +6311,10 @@
         <v>399</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E262" s="2" t="s">
         <v>424</v>
@@ -6376,10 +6328,10 @@
         <v>391</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E263" s="2" t="s">
         <v>424</v>
@@ -6393,7 +6345,7 @@
         <v>411</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>417</v>
@@ -6410,7 +6362,7 @@
         <v>411</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>417</v>
@@ -6427,7 +6379,7 @@
         <v>411</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>417</v>
@@ -6444,7 +6396,7 @@
         <v>400</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>417</v>
@@ -6461,7 +6413,7 @@
         <v>419</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D268" s="2" t="s">
         <v>418</v>
@@ -6478,7 +6430,7 @@
         <v>400</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>417</v>
@@ -6495,7 +6447,7 @@
         <v>419</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>418</v>
@@ -6512,7 +6464,7 @@
         <v>400</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>417</v>
@@ -6529,7 +6481,7 @@
         <v>419</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>418</v>
@@ -6546,13 +6498,13 @@
         <v>267</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6563,10 +6515,10 @@
         <v>401</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E274" s="3" t="s">
         <v>423</v>
@@ -6580,10 +6532,10 @@
         <v>401</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E275" s="3" t="s">
         <v>423</v>
@@ -6597,10 +6549,10 @@
         <v>401</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E276" s="3" t="s">
         <v>423</v>
@@ -6614,10 +6566,10 @@
         <v>401</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E277" s="3" t="s">
         <v>423</v>
@@ -6631,10 +6583,10 @@
         <v>401</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E278" s="3" t="s">
         <v>423</v>
@@ -6648,10 +6600,10 @@
         <v>401</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E279" s="3" t="s">
         <v>423</v>
@@ -6665,10 +6617,10 @@
         <v>389</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E280" s="2" t="s">
         <v>424</v>
@@ -6682,10 +6634,10 @@
         <v>389</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E281" s="2" t="s">
         <v>424</v>
@@ -6699,10 +6651,10 @@
         <v>389</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E282" s="2" t="s">
         <v>424</v>
@@ -6716,7 +6668,7 @@
         <v>402</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>417</v>
@@ -6733,7 +6685,7 @@
         <v>402</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>417</v>
@@ -6750,7 +6702,7 @@
         <v>402</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>417</v>
@@ -6767,7 +6719,7 @@
         <v>402</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>417</v>
@@ -6784,7 +6736,7 @@
         <v>402</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>417</v>
@@ -6801,7 +6753,7 @@
         <v>402</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>417</v>
@@ -6818,7 +6770,7 @@
         <v>402</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>417</v>
@@ -6835,7 +6787,7 @@
         <v>402</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>417</v>
@@ -6852,7 +6804,7 @@
         <v>402</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>417</v>
@@ -6869,7 +6821,7 @@
         <v>402</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>417</v>
@@ -6886,7 +6838,7 @@
         <v>389</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>417</v>
@@ -6903,10 +6855,10 @@
         <v>391</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E294" s="3" t="s">
         <v>422</v>
@@ -6920,10 +6872,10 @@
         <v>391</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E295" s="3" t="s">
         <v>422</v>
@@ -6937,10 +6889,10 @@
         <v>391</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E296" s="3" t="s">
         <v>422</v>
@@ -6954,10 +6906,10 @@
         <v>403</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E297" s="3" t="s">
         <v>422</v>
@@ -6971,10 +6923,10 @@
         <v>403</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E298" s="3" t="s">
         <v>422</v>
@@ -6988,10 +6940,10 @@
         <v>403</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E299" s="3" t="s">
         <v>422</v>
@@ -7005,10 +6957,10 @@
         <v>403</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E300" s="3" t="s">
         <v>422</v>
@@ -7022,10 +6974,10 @@
         <v>403</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E301" s="3" t="s">
         <v>422</v>
@@ -7039,10 +6991,10 @@
         <v>391</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E302" s="2" t="s">
         <v>424</v>
@@ -7056,10 +7008,10 @@
         <v>398</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E303" s="3" t="s">
         <v>423</v>
@@ -7073,10 +7025,10 @@
         <v>389</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E304" s="3" t="s">
         <v>422</v>
@@ -7090,10 +7042,10 @@
         <v>389</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E305" s="3" t="s">
         <v>422</v>
@@ -7107,10 +7059,10 @@
         <v>389</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E306" s="3" t="s">
         <v>422</v>
@@ -7124,10 +7076,10 @@
         <v>389</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E307" s="3" t="s">
         <v>422</v>
@@ -7141,10 +7093,10 @@
         <v>389</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E308" s="3" t="s">
         <v>422</v>
@@ -7158,10 +7110,10 @@
         <v>389</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E309" s="3" t="s">
         <v>422</v>
@@ -7175,10 +7127,10 @@
         <v>391</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E310" s="3" t="s">
         <v>422</v>
@@ -7192,10 +7144,10 @@
         <v>389</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E311" s="2" t="s">
         <v>424</v>
@@ -7209,10 +7161,10 @@
         <v>390</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E312" s="3" t="s">
         <v>422</v>
@@ -7226,10 +7178,10 @@
         <v>390</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E313" s="3" t="s">
         <v>422</v>
@@ -7243,10 +7195,10 @@
         <v>390</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E314" s="3" t="s">
         <v>422</v>
@@ -7260,10 +7212,10 @@
         <v>390</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E315" s="3" t="s">
         <v>422</v>
@@ -7277,10 +7229,10 @@
         <v>390</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E316" s="3" t="s">
         <v>422</v>
@@ -7294,10 +7246,10 @@
         <v>390</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E317" s="3" t="s">
         <v>422</v>
@@ -7311,10 +7263,10 @@
         <v>390</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E318" s="3" t="s">
         <v>422</v>
@@ -7328,10 +7280,10 @@
         <v>404</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E319" s="3" t="s">
         <v>422</v>
@@ -7345,10 +7297,10 @@
         <v>404</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E320" s="3" t="s">
         <v>422</v>
@@ -7362,10 +7314,10 @@
         <v>404</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E321" s="3" t="s">
         <v>422</v>
@@ -7379,10 +7331,10 @@
         <v>404</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E322" s="3" t="s">
         <v>422</v>
@@ -7396,10 +7348,10 @@
         <v>404</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E323" s="3" t="s">
         <v>422</v>
@@ -7413,10 +7365,10 @@
         <v>404</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E324" s="3" t="s">
         <v>422</v>
@@ -7430,10 +7382,10 @@
         <v>404</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E325" s="3" t="s">
         <v>422</v>
@@ -7447,10 +7399,10 @@
         <v>404</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E326" s="3" t="s">
         <v>422</v>
@@ -7464,10 +7416,10 @@
         <v>404</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E327" s="3" t="s">
         <v>422</v>
@@ -7481,10 +7433,10 @@
         <v>404</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E328" s="3" t="s">
         <v>422</v>
@@ -7498,10 +7450,10 @@
         <v>404</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E329" s="3" t="s">
         <v>422</v>
@@ -7515,10 +7467,10 @@
         <v>404</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E330" s="3" t="s">
         <v>422</v>
@@ -7532,10 +7484,10 @@
         <v>404</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E331" s="3" t="s">
         <v>422</v>
@@ -7549,10 +7501,10 @@
         <v>405</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E332" s="3" t="s">
         <v>423</v>
@@ -7566,10 +7518,10 @@
         <v>405</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E333" s="3" t="s">
         <v>423</v>
@@ -7583,10 +7535,10 @@
         <v>405</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E334" s="3" t="s">
         <v>423</v>
@@ -7600,10 +7552,10 @@
         <v>405</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E335" s="3" t="s">
         <v>423</v>
@@ -7617,10 +7569,10 @@
         <v>405</v>
       </c>
       <c r="C336" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E336" s="3" t="s">
         <v>423</v>
@@ -7634,10 +7586,10 @@
         <v>405</v>
       </c>
       <c r="C337" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E337" s="3" t="s">
         <v>423</v>
@@ -7651,10 +7603,10 @@
         <v>389</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E338" s="3" t="s">
         <v>423</v>
@@ -7668,10 +7620,10 @@
         <v>389</v>
       </c>
       <c r="C339" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E339" s="3" t="s">
         <v>423</v>
@@ -7685,10 +7637,10 @@
         <v>389</v>
       </c>
       <c r="C340" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E340" s="3" t="s">
         <v>423</v>
@@ -7702,10 +7654,10 @@
         <v>389</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E341" s="3" t="s">
         <v>423</v>
@@ -7719,7 +7671,7 @@
         <v>406</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D342" s="2" t="s">
         <v>417</v>
@@ -7736,7 +7688,7 @@
         <v>420</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D343" s="2" t="s">
         <v>108</v>
@@ -7753,7 +7705,7 @@
         <v>406</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>417</v>
@@ -7770,7 +7722,7 @@
         <v>420</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D345" s="2" t="s">
         <v>108</v>
@@ -7787,7 +7739,7 @@
         <v>406</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D346" s="2" t="s">
         <v>417</v>
@@ -7804,7 +7756,7 @@
         <v>406</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D347" s="2" t="s">
         <v>417</v>
@@ -7821,7 +7773,7 @@
         <v>406</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D348" s="2" t="s">
         <v>418</v>
@@ -7838,7 +7790,7 @@
         <v>406</v>
       </c>
       <c r="C349" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D349" s="2" t="s">
         <v>417</v>
@@ -7855,7 +7807,7 @@
         <v>406</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D350" s="2" t="s">
         <v>417</v>
@@ -7872,7 +7824,7 @@
         <v>406</v>
       </c>
       <c r="C351" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D351" s="2" t="s">
         <v>417</v>
@@ -7889,7 +7841,7 @@
         <v>406</v>
       </c>
       <c r="C352" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>418</v>
@@ -7906,7 +7858,7 @@
         <v>406</v>
       </c>
       <c r="C353" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D353" s="2" t="s">
         <v>418</v>
@@ -7923,7 +7875,7 @@
         <v>406</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D354" s="2" t="s">
         <v>418</v>
@@ -7940,7 +7892,7 @@
         <v>406</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D355" s="2" t="s">
         <v>417</v>
@@ -7957,7 +7909,7 @@
         <v>406</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D356" s="2" t="s">
         <v>417</v>
@@ -7974,7 +7926,7 @@
         <v>406</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D357" s="2" t="s">
         <v>417</v>
@@ -7991,7 +7943,7 @@
         <v>412</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D358" s="2" t="s">
         <v>417</v>
@@ -8008,7 +7960,7 @@
         <v>412</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D359" s="2" t="s">
         <v>417</v>
@@ -8025,10 +7977,10 @@
         <v>393</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E360" s="3" t="s">
         <v>422</v>
@@ -8042,10 +7994,10 @@
         <v>393</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E361" s="3" t="s">
         <v>422</v>
@@ -8059,10 +8011,10 @@
         <v>389</v>
       </c>
       <c r="C362" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E362" s="3" t="s">
         <v>423</v>
@@ -8076,10 +8028,10 @@
         <v>389</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E363" s="3" t="s">
         <v>423</v>
@@ -8093,10 +8045,10 @@
         <v>389</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E364" s="3" t="s">
         <v>423</v>
@@ -8110,10 +8062,10 @@
         <v>389</v>
       </c>
       <c r="C365" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E365" s="3" t="s">
         <v>423</v>
@@ -8127,10 +8079,10 @@
         <v>389</v>
       </c>
       <c r="C366" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E366" s="3" t="s">
         <v>423</v>
@@ -8144,10 +8096,10 @@
         <v>389</v>
       </c>
       <c r="C367" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E367" s="3" t="s">
         <v>422</v>
@@ -8161,10 +8113,10 @@
         <v>389</v>
       </c>
       <c r="C368" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E368" s="3" t="s">
         <v>422</v>
@@ -8178,10 +8130,10 @@
         <v>389</v>
       </c>
       <c r="C369" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E369" s="3" t="s">
         <v>422</v>
@@ -8195,10 +8147,10 @@
         <v>389</v>
       </c>
       <c r="C370" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E370" s="3" t="s">
         <v>422</v>
@@ -8212,10 +8164,10 @@
         <v>389</v>
       </c>
       <c r="C371" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E371" s="3" t="s">
         <v>422</v>
@@ -8229,10 +8181,10 @@
         <v>389</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E372" s="2" t="s">
         <v>424</v>
@@ -8246,7 +8198,7 @@
         <v>388</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>417</v>
@@ -8263,7 +8215,7 @@
         <v>388</v>
       </c>
       <c r="C374" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D374" s="2" t="s">
         <v>417</v>
@@ -8280,7 +8232,7 @@
         <v>388</v>
       </c>
       <c r="C375" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D375" s="2" t="s">
         <v>417</v>
@@ -8297,7 +8249,7 @@
         <v>413</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D376" s="2" t="s">
         <v>418</v>
@@ -8314,7 +8266,7 @@
         <v>413</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D377" s="2" t="s">
         <v>418</v>
@@ -8331,7 +8283,7 @@
         <v>413</v>
       </c>
       <c r="C378" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D378" s="2" t="s">
         <v>418</v>
@@ -8348,7 +8300,7 @@
         <v>388</v>
       </c>
       <c r="C379" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D379" s="2" t="s">
         <v>417</v>
@@ -8365,7 +8317,7 @@
         <v>413</v>
       </c>
       <c r="C380" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D380" s="2" t="s">
         <v>418</v>
@@ -8382,7 +8334,7 @@
         <v>388</v>
       </c>
       <c r="C381" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D381" s="2" t="s">
         <v>417</v>
@@ -8399,7 +8351,7 @@
         <v>388</v>
       </c>
       <c r="C382" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D382" s="2" t="s">
         <v>417</v>
@@ -8416,7 +8368,7 @@
         <v>413</v>
       </c>
       <c r="C383" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D383" s="2" t="s">
         <v>418</v>
@@ -8433,7 +8385,7 @@
         <v>388</v>
       </c>
       <c r="C384" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D384" s="2" t="s">
         <v>417</v>
@@ -8450,7 +8402,7 @@
         <v>413</v>
       </c>
       <c r="C385" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D385" s="2" t="s">
         <v>418</v>
@@ -8467,7 +8419,7 @@
         <v>388</v>
       </c>
       <c r="C386" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D386" s="2" t="s">
         <v>417</v>
@@ -8484,7 +8436,7 @@
         <v>388</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D387" s="2" t="s">
         <v>417</v>
@@ -8501,7 +8453,7 @@
         <v>388</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D388" s="2" t="s">
         <v>417</v>
@@ -8518,10 +8470,10 @@
         <v>389</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E389" s="2" t="s">
         <v>424</v>
@@ -8535,10 +8487,10 @@
         <v>389</v>
       </c>
       <c r="C390" s="2" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E390" s="2" t="s">
         <v>424</v>
@@ -8552,10 +8504,10 @@
         <v>390</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E391" s="3" t="s">
         <v>422</v>
@@ -8569,10 +8521,10 @@
         <v>390</v>
       </c>
       <c r="C392" s="2" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="D392" s="2" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E392" s="3" t="s">
         <v>422</v>

</xml_diff>

<commit_message>
Fix bugs and add docs for functions
</commit_message>
<xml_diff>
--- a/Columns.xlsx
+++ b/Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\DR_mod\DR_Potentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7493B726-FFA1-4514-BDF5-FBDC1D44FCBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15CB286-1DDA-45E0-B219-ADC5C3A0D871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix bugs in columns mapping
</commit_message>
<xml_diff>
--- a/Columns.xlsx
+++ b/Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\DR_mod\DR_Potentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15CB286-1DDA-45E0-B219-ADC5C3A0D871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E5DE4-22FE-4729-B76C-3FBA282A4647}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,7 +3903,7 @@
         <v>428</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3920,7 +3920,7 @@
         <v>428</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3937,7 +3937,7 @@
         <v>428</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3954,7 +3954,7 @@
         <v>428</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,7 +3971,7 @@
         <v>428</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,7 +3988,7 @@
         <v>428</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>428</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
         <v>428</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4107,7 +4107,7 @@
         <v>428</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,7 +4124,7 @@
         <v>428</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4141,7 +4141,7 @@
         <v>428</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -6283,7 +6283,7 @@
         <v>428</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6300,7 +6300,7 @@
         <v>428</v>
       </c>
       <c r="E261" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6317,7 +6317,7 @@
         <v>428</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -7770,7 +7770,7 @@
         <v>342</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>430</v>
@@ -7838,7 +7838,7 @@
         <v>346</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>430</v>
@@ -7855,7 +7855,7 @@
         <v>347</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>430</v>
@@ -7872,7 +7872,7 @@
         <v>348</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>430</v>

</xml_diff>